<commit_message>
update Assigment1.R - 1st idea of analysis
</commit_message>
<xml_diff>
--- a/Assignment1.xlsx
+++ b/Assignment1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/aoi_kawahara_student_kuleuven_be/Documents/Leuven/04_Event History Analysis/Excersice/Workplace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/aoi_kawahara_student_kuleuven_be/Documents/Leuven/04_Event History Analysis/Assignment/Workplace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCF6A15B-71F0-9C43-83AC-E2F9F5C8591F}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADFD7FEE-8281-AD47-89AF-70A52E20E646}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="1120" windowWidth="17480" windowHeight="16260" xr2:uid="{5E45D5F4-AF93-E849-8494-C63BC031ADCC}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="23220" windowHeight="18380" xr2:uid="{5E45D5F4-AF93-E849-8494-C63BC031ADCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,16 +50,20 @@
     <t>Censoring</t>
   </si>
   <si>
-    <t>Discrete-time Hazard</t>
+    <t>Survivor function</t>
   </si>
   <si>
-    <t>Conditional probability of survival</t>
+    <t>Conditional probability
+of survival</t>
   </si>
   <si>
-    <t>number still having 2 children at the beginning of the interval according to the survivor function</t>
+    <t>Discrete-time
+Hazard</t>
   </si>
   <si>
-    <t>Survivor function</t>
+    <t>Number still having 2 children
+at the beginning of the interval
+according to the survivor function</t>
   </si>
 </sst>
 </file>
@@ -67,14 +71,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -86,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -94,14 +105,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,6 +1204,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1314,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42215F8A-3C11-9443-BBFD-9D3FE740C475}">
-  <dimension ref="B2:I22"/>
+  <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,654 +1537,655 @@
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" s="16" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3">
+      <c r="B3" s="9">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>1160</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>20</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <f>C3-D3-C4</f>
         <v>84</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="11">
         <f>D3/C3</f>
         <v>1.7241379310344827E-2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="11">
         <f>1-F3</f>
         <v>0.98275862068965514</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="11">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="12">
         <f>H3*C3</f>
         <v>1160</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1056</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>56</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f t="shared" ref="E4:E22" si="0">C4-D4-C5</f>
         <v>85</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <f t="shared" ref="F4:F22" si="1">D4/C4</f>
         <v>5.3030303030303032E-2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <f>1-F4</f>
         <v>0.94696969696969702</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <f>H3*G3</f>
         <v>0.98275862068965514</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <f>H4*C4</f>
         <v>1037.7931034482758</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>915</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>86</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>9.3989071038251368E-2</v>
       </c>
-      <c r="G5" s="1">
-        <f t="shared" ref="G4:G22" si="2">1-F5</f>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G22" si="2">1-F5</f>
         <v>0.90601092896174862</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <f>H4*G4</f>
         <v>0.93064263322884011</v>
       </c>
-      <c r="I5" s="2">
-        <f t="shared" ref="I4:I22" si="3">H5*C5</f>
+      <c r="I5" s="4">
+        <f t="shared" ref="I5:I22" si="3">H5*C5</f>
         <v>851.53800940438873</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>746</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>60</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>8.0428954423592491E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <f t="shared" si="2"/>
         <v>0.91957104557640745</v>
       </c>
-      <c r="H6" s="1">
-        <f t="shared" ref="H5:H22" si="4">H5*G5</f>
+      <c r="H6" s="2">
+        <f t="shared" ref="H6:H22" si="4">H5*G5</f>
         <v>0.84317239666306931</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <f t="shared" si="3"/>
         <v>629.00660791064968</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>614</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>44</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>7.1661237785016291E-2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
         <v>0.92833876221498368</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <f t="shared" si="4"/>
         <v>0.77535692240062404</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <f t="shared" si="3"/>
         <v>476.06915035398316</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8">
+      <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>506</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>32</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>6.3241106719367585E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <f t="shared" si="2"/>
         <v>0.93675889328063244</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <f t="shared" si="4"/>
         <v>0.71979388561621449</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="4">
         <f t="shared" si="3"/>
         <v>364.21570612180454</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9">
+      <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>421</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>3.3254156769596199E-2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <f t="shared" si="2"/>
         <v>0.9667458432304038</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <f t="shared" si="4"/>
         <v>0.67427332368001125</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="4">
         <f t="shared" si="3"/>
         <v>283.86906926928475</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10">
+      <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>353</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>3.39943342776204E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <f t="shared" si="2"/>
         <v>0.96600566572237956</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <f t="shared" si="4"/>
         <v>0.65185093286879947</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="4">
         <f t="shared" si="3"/>
         <v>230.10337930268622</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11">
+      <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>286</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>6</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>2.097902097902098E-2</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <f t="shared" si="2"/>
         <v>0.97902097902097907</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <f t="shared" si="4"/>
         <v>0.6296916943576788</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="4">
         <f t="shared" si="3"/>
         <v>180.09182458629613</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12">
+      <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>238</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>1.680672268907563E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <f t="shared" si="2"/>
         <v>0.98319327731092432</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <f t="shared" si="4"/>
         <v>0.61648137909143386</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="4">
         <f t="shared" si="3"/>
         <v>146.72256822376127</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13">
+      <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>194</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>2.0618556701030927E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <f t="shared" si="2"/>
         <v>0.97938144329896903</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <f t="shared" si="4"/>
         <v>0.60612034751006516</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="4">
         <f t="shared" si="3"/>
         <v>117.58734741695264</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14">
+      <c r="B14" s="3">
         <v>11</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>139</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>2.1582733812949641E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
         <v>0.97841726618705038</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <f t="shared" si="4"/>
         <v>0.59362302075728024</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="4">
         <f t="shared" si="3"/>
         <v>82.513599885261954</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15">
+      <c r="B15" s="3">
         <v>12</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>91</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>1.098901098901099E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <f t="shared" si="2"/>
         <v>0.98901098901098905</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <f t="shared" si="4"/>
         <v>0.5808110131150368</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="4">
         <f t="shared" si="3"/>
         <v>52.853802193468347</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16">
+      <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>58</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <f t="shared" si="1"/>
         <v>1.7241379310344827E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <f t="shared" si="2"/>
         <v>0.98275862068965514</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <f t="shared" si="4"/>
         <v>0.57442847450937706</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="4">
         <f t="shared" si="3"/>
         <v>33.316851521543867</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17">
+      <c r="B17" s="3">
         <v>14</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>37</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <f t="shared" si="4"/>
         <v>0.56452453529369817</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="4">
         <f t="shared" si="3"/>
         <v>20.887407805866832</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18">
+      <c r="B18" s="3">
         <v>15</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>28</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <f t="shared" si="4"/>
         <v>0.56452453529369817</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="4">
         <f t="shared" si="3"/>
         <v>15.806686988223548</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19">
+      <c r="B19" s="3">
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>15</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <f t="shared" si="4"/>
         <v>0.56452453529369817</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="4">
         <f t="shared" si="3"/>
         <v>8.4678680294054729</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20">
+      <c r="B20" s="3">
         <v>17</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <f t="shared" si="4"/>
         <v>0.56452453529369817</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="4">
         <f t="shared" si="3"/>
         <v>4.5161962823495854</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21">
+      <c r="B21" s="3">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <f t="shared" si="4"/>
         <v>0.56452453529369817</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="4">
         <f t="shared" si="3"/>
         <v>2.2580981411747927</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22">
+    <row r="22" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
         <v>19</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>0</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="7">
         <f t="shared" si="4"/>
         <v>0.56452453529369817</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="8">
         <f t="shared" si="3"/>
         <v>0.56452453529369817</v>
       </c>

</xml_diff>

<commit_message>
update Assigment1.R - add step function
</commit_message>
<xml_diff>
--- a/Assignment1.xlsx
+++ b/Assignment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/aoi_kawahara_student_kuleuven_be/Documents/Leuven/04_Event History Analysis/Assignment/Workplace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADFD7FEE-8281-AD47-89AF-70A52E20E646}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1809B47-2B4D-F641-BE1C-820BA76497A2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="23220" windowHeight="18380" xr2:uid="{5E45D5F4-AF93-E849-8494-C63BC031ADCC}"/>
   </bookViews>
@@ -1528,7 +1528,7 @@
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add Assignment2 and resource
</commit_message>
<xml_diff>
--- a/Assignment1.xlsx
+++ b/Assignment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/aoi_kawahara_student_kuleuven_be/Documents/Leuven/04_Event History Analysis/Assignment/Workplace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1809B47-2B4D-F641-BE1C-820BA76497A2}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11168598-3BFB-694E-B8E9-00D7C1A2D37F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="23220" windowHeight="18380" xr2:uid="{5E45D5F4-AF93-E849-8494-C63BC031ADCC}"/>
   </bookViews>
@@ -1528,7 +1528,7 @@
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1647,7 +1647,7 @@
         <v>83</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f>D5/C5</f>
         <v>9.3989071038251368E-2</v>
       </c>
       <c r="G5" s="2">
@@ -1713,7 +1713,7 @@
         <v>7.1661237785016291E-2</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="2"/>
+        <f>1-F7</f>
         <v>0.92833876221498368</v>
       </c>
       <c r="H7" s="2">

</xml_diff>

<commit_message>
update Assignment2.R - partial residuals
</commit_message>
<xml_diff>
--- a/Assignment1.xlsx
+++ b/Assignment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/aoi_kawahara_student_kuleuven_be/Documents/Leuven/04_Event History Analysis/Assignment/Workplace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11168598-3BFB-694E-B8E9-00D7C1A2D37F}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{C8013863-9298-9A4C-A70C-ACC9861B99CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80547578-A2BC-5F4B-8C73-0A4488C31EAD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="23220" windowHeight="18380" xr2:uid="{5E45D5F4-AF93-E849-8494-C63BC031ADCC}"/>
   </bookViews>
@@ -1651,7 +1651,7 @@
         <v>9.3989071038251368E-2</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G22" si="2">1-F5</f>
+        <f>1-F5</f>
         <v>0.90601092896174862</v>
       </c>
       <c r="H5" s="2">
@@ -1659,7 +1659,7 @@
         <v>0.93064263322884011</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I22" si="3">H5*C5</f>
+        <f t="shared" ref="I5:I22" si="2">H5*C5</f>
         <v>851.53800940438873</v>
       </c>
     </row>
@@ -1678,11 +1678,11 @@
         <v>72</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f>D6/C6</f>
         <v>8.0428954423592491E-2</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G5:G22" si="3">1-F6</f>
         <v>0.91957104557640745</v>
       </c>
       <c r="H6" s="2">
@@ -1690,7 +1690,7 @@
         <v>0.84317239666306931</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>629.00660791064968</v>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
         <v>0.77535692240062404</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>476.06915035398316</v>
       </c>
     </row>
@@ -1744,7 +1744,7 @@
         <v>6.3241106719367585E-2</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.93675889328063244</v>
       </c>
       <c r="H8" s="2">
@@ -1752,7 +1752,7 @@
         <v>0.71979388561621449</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>364.21570612180454</v>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
         <v>3.3254156769596199E-2</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.9667458432304038</v>
       </c>
       <c r="H9" s="2">
@@ -1783,7 +1783,7 @@
         <v>0.67427332368001125</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>283.86906926928475</v>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
         <v>3.39943342776204E-2</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.96600566572237956</v>
       </c>
       <c r="H10" s="2">
@@ -1814,7 +1814,7 @@
         <v>0.65185093286879947</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>230.10337930268622</v>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
         <v>2.097902097902098E-2</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.97902097902097907</v>
       </c>
       <c r="H11" s="2">
@@ -1845,7 +1845,7 @@
         <v>0.6296916943576788</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>180.09182458629613</v>
       </c>
     </row>
@@ -1868,7 +1868,7 @@
         <v>1.680672268907563E-2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.98319327731092432</v>
       </c>
       <c r="H12" s="2">
@@ -1876,7 +1876,7 @@
         <v>0.61648137909143386</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>146.72256822376127</v>
       </c>
     </row>
@@ -1899,7 +1899,7 @@
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.97938144329896903</v>
       </c>
       <c r="H13" s="2">
@@ -1907,7 +1907,7 @@
         <v>0.60612034751006516</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>117.58734741695264</v>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
         <v>2.1582733812949641E-2</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.97841726618705038</v>
       </c>
       <c r="H14" s="2">
@@ -1938,7 +1938,7 @@
         <v>0.59362302075728024</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>82.513599885261954</v>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
         <v>1.098901098901099E-2</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.98901098901098905</v>
       </c>
       <c r="H15" s="2">
@@ -1969,7 +1969,7 @@
         <v>0.5808110131150368</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>52.853802193468347</v>
       </c>
     </row>
@@ -1992,7 +1992,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.98275862068965514</v>
       </c>
       <c r="H16" s="2">
@@ -2000,7 +2000,7 @@
         <v>0.57442847450937706</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>33.316851521543867</v>
       </c>
     </row>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H17" s="2">
@@ -2031,7 +2031,7 @@
         <v>0.56452453529369817</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20.887407805866832</v>
       </c>
     </row>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H18" s="2">
@@ -2062,7 +2062,7 @@
         <v>0.56452453529369817</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15.806686988223548</v>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H19" s="2">
@@ -2093,7 +2093,7 @@
         <v>0.56452453529369817</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8.4678680294054729</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H20" s="2">
@@ -2124,7 +2124,7 @@
         <v>0.56452453529369817</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.5161962823495854</v>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H21" s="2">
@@ -2155,7 +2155,7 @@
         <v>0.56452453529369817</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.2580981411747927</v>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H22" s="7">
@@ -2186,7 +2186,7 @@
         <v>0.56452453529369817</v>
       </c>
       <c r="I22" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.56452453529369817</v>
       </c>
     </row>

</xml_diff>